<commit_message>
Change text for German labs
Minor changes to a text file for German labs following feedback
</commit_message>
<xml_diff>
--- a/measures/4 site-specific measures for data collection/Gast, Richter, & Benedict/text/instructions.xlsx
+++ b/measures/4 site-specific measures for data collection/Gast, Richter, & Benedict/text/instructions.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20351"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nutzer\sciebo\EC\EC\Replication Surveillance\translation and pretesting package to be sent to sites\translation Team1\German_translated\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmoranyo\Documents\GitHub\unconscious-ec-RRR\measures\4 site-specific measures for data collection\Hütter\text\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA83803-D878-48F8-8C2E-8D7B61F512B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945"/>
   </bookViews>
   <sheets>
     <sheet name="instructions" sheetId="1" r:id="rId1"/>
@@ -63,21 +62,8 @@
 Beachten Sie, dass es keine richtigen oder falschen Antworten gibt. </t>
   </si>
   <si>
-    <t xml:space="preserve">Als Nächstes werden Ihnen 30 Paare aus Ziel- und Füll-Wesen aus der Überwachungsaufgabe gezeigt und wir bitten Sie anzugeben, welches Sie lieber mögen.  
-Sie brauchen keinen Grund, um eines lieber als das andere zu mögen, sagen Sie uns einfach Ihr Bauchgefühl.
-Uns interessiert, ob die Angenehmheit oder Unangenehmheit der Wesen die Fähigkeit beeinflusst, sie aufmerksam zu beobachten und schnell auf sie zu reagieren. Daher benötigen wir Ihre Angabe, welches Sie lieber mögen.  
-Nicht vergessen: Sie brauchen keinen Grund, um eines lieber als das andere zu mögen, also folgen Sie einfach Ihrem Bauchgefühl. Bitte antworten Sie zügig.
-Drücken Sie die Leertaste, um fortzufahren. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Zuletzt werden wir Ihnen eine Reihe von kurzen Fragen stellen und danach wird die Studie beendet sein. 
 Drücken Sie die Leertaste, um fortzufahren. </t>
-  </si>
-  <si>
-    <t>Stellen Sie sich vor, Sie wären ein Sicherheitsmann der auffällige Aktivitäten in einem Unternehmen überwacht. Ihre Aufgabe erfordert ständige Aufmerksamkeit und schnelle Reaktionen, wenn etwas Verdächtiges passiert.   
-Wir untersuchen in unserem Labor Aufmerksamkeit und Reaktionsgeschwindigkeit und in diesem Experiment bitten wir Sie, die Rolle des Sicherheitsmannes zu spielen.  
-Genauer werden Sie eine Reihe von Dingen auf dem Computerbildschirm beobachten und so schnell wie möglich reagieren, indem Sie die Leertaste drücken, wenn ein Zielgegenstand auftaucht.  
-Drücken Sie die Leertaste, um fortzufahren.</t>
   </si>
   <si>
     <t>Der Zielgegenstand wird im Laufe des Experiments einige Male zufällig auftauchen. Der Zielgegenstand kann als Bild oder als Name auftauchen. Also seien Sie unbedingt die ganze Zeit über aufmerksam und konzentrieren Sie sich auf den Bildschrim, denn Sie wissen nie, wann der Zielgegenstand auftauchen wird.   
@@ -86,11 +72,24 @@
 Der Zielgegenstand kann irgendwo auf dem Bildschirm auftauchen und er kann auch mit anderen Bildern auftreten. Also drücken Sie jedes Mal, wenn Sie ein Zielbild oder einen Zielnamen irgendwo auf dem Bildschrim sehen, die Leertaste.  
 Drücken Sie die Leertaste, um fortzufahren.</t>
   </si>
+  <si>
+    <t>Stellen Sie sich vor, Sie wären ein Sicherheitsperson der auffällige Aktivitäten in einem Unternehmen überwacht. Ihre Aufgabe erfordert ständige Aufmerksamkeit und schnelle Reaktionen, wenn etwas Verdächtiges passiert.   
+Wir untersuchen in unserem Labor Aufmerksamkeit und Reaktionsgeschwindigkeit und in diesem Experiment bitten wir Sie, die Rolle des Sicherheitsmannes zu spielen.  
+Genauer werden Sie eine Reihe von Dingen auf dem Computerbildschirm beobachten und so schnell wie möglich reagieren, indem Sie die Leertaste drücken, wenn ein Zielgegenstand auftaucht.  
+Drücken Sie die Leertaste, um fortzufahren.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Als Nächstes werden Ihnen 30 Paare aus Ziel- und Füll-Wesen aus der Überwachungsaufgabe gezeigt und wir bitten Sie anzugeben, welches Sie lieber mögen.  
+Sie brauchen keinen Grund, um eines lieber als das andere zu mögen. Teilen Sie uns einfach mit, was Ihr Bauchgefühl ist.
+Uns interessiert, ob die Angenehmheit oder Unangenehmheit der Wesen die Fähigkeit beeinflusst, sie aufmerksam zu beobachten und schnell auf sie zu reagieren. Daher benötigen wir Ihre Angabe, welches Sie lieber mögen.  
+Nicht vergessen: Sie brauchen keinen Grund, um eines lieber als das andere zu mögen, also folgen Sie einfach Ihrem Bauchgefühl. Bitte antworten Sie zügig.
+Drücken Sie die Leertaste, um fortzufahren. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -604,48 +603,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -956,14 +955,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="89.375" customWidth="1"/>
   </cols>
@@ -985,7 +984,7 @@
     </row>
     <row r="4" spans="1:1" ht="297" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="230.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1010,7 +1009,7 @@
     </row>
     <row r="9" spans="1:1" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="126" x14ac:dyDescent="0.25">
@@ -1020,7 +1019,7 @@
     </row>
     <row r="11" spans="1:1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="47.25" x14ac:dyDescent="0.25">

</xml_diff>